<commit_message>
add doc review cases
</commit_message>
<xml_diff>
--- a/source.xlsx
+++ b/source.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\excel_generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HarryQian\Desktop\excel_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="20490" windowHeight="7760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Scope" sheetId="2" r:id="rId1"/>
     <sheet name="Details" sheetId="3" r:id="rId2"/>
     <sheet name="binary" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="132">
   <si>
     <t>Test Items</t>
   </si>
@@ -590,24 +590,32 @@
   </si>
   <si>
     <t>APP-USB0-CV_Test_Device</t>
+  </si>
+  <si>
+    <t>document  review</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>document_review</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -639,7 +647,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -647,8 +655,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -702,7 +717,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -754,11 +769,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -824,6 +850,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -865,7 +892,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1149,16 +1176,16 @@
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="8" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="35.81640625" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" style="8" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" customWidth="1"/>
     <col min="9" max="9" width="7" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1166,10 +1193,10 @@
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31"/>
+      <c r="C1" s="32"/>
       <c r="D1" s="18" t="s">
         <v>42</v>
       </c>
@@ -1192,10 +1219,10 @@
       <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="35">
-        <v>1</v>
-      </c>
-      <c r="B2" s="33" t="s">
+      <c r="A2" s="36">
+        <v>1</v>
+      </c>
+      <c r="B2" s="34" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1203,153 +1230,153 @@
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
-      <c r="F2" s="39">
+      <c r="F2" s="40">
         <v>4</v>
       </c>
       <c r="G2" s="17"/>
-      <c r="H2" s="38">
+      <c r="H2" s="39">
         <v>4</v>
       </c>
-      <c r="I2" s="39">
+      <c r="I2" s="40">
         <v>4</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="33"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
-      <c r="F3" s="39"/>
+      <c r="F3" s="40"/>
       <c r="G3" s="17"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="40"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="33"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="39"/>
+      <c r="F4" s="40"/>
       <c r="G4" s="17"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="40"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
+    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.25">
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
-      <c r="F5" s="39"/>
+      <c r="F5" s="40"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="40"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="2" t="s">
         <v>62</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="39"/>
+      <c r="F6" s="40"/>
       <c r="G6" s="17"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="40"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
-      <c r="B7" s="35"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
-      <c r="F7" s="39"/>
+      <c r="F7" s="40"/>
       <c r="G7" s="17"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="40"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
-      <c r="B8" s="35"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="39"/>
+      <c r="F8" s="40"/>
       <c r="G8" s="17"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="40"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35"/>
+      <c r="A9" s="36"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="2" t="s">
         <v>64</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
-      <c r="F9" s="39"/>
+      <c r="F9" s="40"/>
       <c r="G9" s="17"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="40"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
+    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.25">
+      <c r="A10" s="36"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="39"/>
+      <c r="F10" s="40"/>
       <c r="G10" s="16"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="39"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
-      <c r="B11" s="35"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="40"/>
+    </row>
+    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.25">
+      <c r="A11" s="36"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
-      <c r="F11" s="39"/>
+      <c r="F11" s="40"/>
       <c r="G11" s="16"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="39"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="35">
+      <c r="H11" s="39"/>
+      <c r="I11" s="40"/>
+    </row>
+    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.25">
+      <c r="A12" s="36">
         <v>2</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="34" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1357,139 +1384,139 @@
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
-      <c r="F12" s="39">
+      <c r="F12" s="40">
         <v>10</v>
       </c>
       <c r="G12" s="16"/>
-      <c r="H12" s="38">
+      <c r="H12" s="39">
         <v>10</v>
       </c>
-      <c r="I12" s="39">
+      <c r="I12" s="40">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
-      <c r="F13" s="39"/>
+      <c r="F13" s="40"/>
       <c r="G13" s="10"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="40"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="39"/>
+      <c r="F14" s="40"/>
       <c r="G14" s="10"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="40"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
-      <c r="F15" s="39"/>
+      <c r="F15" s="40"/>
       <c r="G15" s="10"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="40"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="39"/>
+      <c r="F16" s="40"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="40"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="36"/>
       <c r="C17" s="5" t="s">
         <v>53</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="39"/>
+      <c r="F17" s="40"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="40"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="36"/>
       <c r="C18" s="6" t="s">
         <v>54</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
-      <c r="F18" s="39"/>
+      <c r="F18" s="40"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="40"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6" t="s">
         <v>55</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
-      <c r="F19" s="39"/>
+      <c r="F19" s="40"/>
       <c r="G19" s="10"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="40"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="35"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
-      <c r="F20" s="39"/>
+      <c r="F20" s="40"/>
       <c r="G20" s="10"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="40"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
-      <c r="B21" s="35"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="36"/>
       <c r="C21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
-      <c r="F21" s="39"/>
+      <c r="F21" s="40"/>
       <c r="G21" s="10"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="40"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="35">
+      <c r="A22" s="36">
         <v>3</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="33" t="s">
         <v>83</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1510,14 +1537,14 @@
       <c r="H22" s="10">
         <v>0.25</v>
       </c>
-      <c r="I22" s="39">
+      <c r="I22" s="40">
         <f>SUM(F22:F42)</f>
         <v>9.3000000000000025</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
-      <c r="B23" s="32"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="3" t="s">
         <v>8</v>
       </c>
@@ -1536,11 +1563,11 @@
       <c r="H23" s="10">
         <v>0.25</v>
       </c>
-      <c r="I23" s="39"/>
+      <c r="I23" s="40"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
-      <c r="B24" s="32"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="33"/>
       <c r="C24" s="3" t="s">
         <v>6</v>
       </c>
@@ -1559,11 +1586,11 @@
       <c r="H24" s="10">
         <v>0.25</v>
       </c>
-      <c r="I24" s="39"/>
+      <c r="I24" s="40"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
-      <c r="B25" s="32"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="33"/>
       <c r="C25" s="3" t="s">
         <v>9</v>
       </c>
@@ -1582,11 +1609,11 @@
       <c r="H25" s="10">
         <v>0.25</v>
       </c>
-      <c r="I25" s="39"/>
+      <c r="I25" s="40"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
-      <c r="B26" s="32"/>
+      <c r="A26" s="36"/>
+      <c r="B26" s="33"/>
       <c r="C26" s="3" t="s">
         <v>10</v>
       </c>
@@ -1605,11 +1632,11 @@
       <c r="H26" s="10">
         <v>0.25</v>
       </c>
-      <c r="I26" s="39"/>
+      <c r="I26" s="40"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
-      <c r="B27" s="32"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="33"/>
       <c r="C27" s="3" t="s">
         <v>29</v>
       </c>
@@ -1628,11 +1655,11 @@
       <c r="H27" s="10">
         <v>0.25</v>
       </c>
-      <c r="I27" s="39"/>
+      <c r="I27" s="40"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
-      <c r="B28" s="32"/>
+      <c r="A28" s="36"/>
+      <c r="B28" s="33"/>
       <c r="C28" s="3" t="s">
         <v>75</v>
       </c>
@@ -1645,11 +1672,11 @@
       <c r="H28" s="22">
         <v>0.25</v>
       </c>
-      <c r="I28" s="39"/>
+      <c r="I28" s="40"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
-      <c r="B29" s="32"/>
+      <c r="A29" s="36"/>
+      <c r="B29" s="33"/>
       <c r="C29" s="9" t="s">
         <v>41</v>
       </c>
@@ -1668,11 +1695,11 @@
       <c r="H29" s="11">
         <v>0.2</v>
       </c>
-      <c r="I29" s="39"/>
+      <c r="I29" s="40"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
-      <c r="B30" s="32"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="2" t="s">
         <v>3</v>
       </c>
@@ -1691,11 +1718,11 @@
       <c r="H30" s="11">
         <v>0.2</v>
       </c>
-      <c r="I30" s="39"/>
+      <c r="I30" s="40"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
-      <c r="B31" s="32"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="33"/>
       <c r="C31" s="2" t="s">
         <v>4</v>
       </c>
@@ -1714,11 +1741,11 @@
       <c r="H31" s="11">
         <v>0.2</v>
       </c>
-      <c r="I31" s="39"/>
+      <c r="I31" s="40"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="35"/>
-      <c r="B32" s="32"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="33"/>
       <c r="C32" s="2" t="s">
         <v>5</v>
       </c>
@@ -1737,11 +1764,11 @@
       <c r="H32" s="11">
         <v>0.2</v>
       </c>
-      <c r="I32" s="39"/>
+      <c r="I32" s="40"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
-      <c r="B33" s="32"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="33"/>
       <c r="C33" s="2" t="s">
         <v>7</v>
       </c>
@@ -1760,11 +1787,11 @@
       <c r="H33" s="11">
         <v>0.4</v>
       </c>
-      <c r="I33" s="39"/>
+      <c r="I33" s="40"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="35"/>
-      <c r="B34" s="32"/>
+      <c r="A34" s="36"/>
+      <c r="B34" s="33"/>
       <c r="C34" s="2" t="s">
         <v>12</v>
       </c>
@@ -1783,11 +1810,11 @@
       <c r="H34" s="11">
         <v>0.4</v>
       </c>
-      <c r="I34" s="39"/>
+      <c r="I34" s="40"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="35"/>
-      <c r="B35" s="32"/>
+      <c r="A35" s="36"/>
+      <c r="B35" s="33"/>
       <c r="C35" s="2" t="s">
         <v>13</v>
       </c>
@@ -1806,11 +1833,11 @@
       <c r="H35" s="11">
         <v>0.2</v>
       </c>
-      <c r="I35" s="39"/>
+      <c r="I35" s="40"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
-      <c r="B36" s="32"/>
+      <c r="A36" s="36"/>
+      <c r="B36" s="33"/>
       <c r="C36" s="2" t="s">
         <v>30</v>
       </c>
@@ -1829,11 +1856,11 @@
       <c r="H36" s="11">
         <v>0.2</v>
       </c>
-      <c r="I36" s="39"/>
+      <c r="I36" s="40"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
-      <c r="B37" s="32"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="33"/>
       <c r="C37" s="2" t="s">
         <v>27</v>
       </c>
@@ -1852,11 +1879,11 @@
       <c r="H37" s="11">
         <v>0.2</v>
       </c>
-      <c r="I37" s="39"/>
+      <c r="I37" s="40"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="35"/>
-      <c r="B38" s="32"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="33"/>
       <c r="C38" s="2" t="s">
         <v>31</v>
       </c>
@@ -1875,11 +1902,11 @@
       <c r="H38" s="11">
         <v>0.2</v>
       </c>
-      <c r="I38" s="39"/>
+      <c r="I38" s="40"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="35"/>
-      <c r="B39" s="32"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="33"/>
       <c r="C39" s="6" t="s">
         <v>38</v>
       </c>
@@ -1898,11 +1925,11 @@
       <c r="H39" s="11">
         <v>0.2</v>
       </c>
-      <c r="I39" s="39"/>
+      <c r="I39" s="40"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="35"/>
-      <c r="B40" s="32"/>
+      <c r="A40" s="36"/>
+      <c r="B40" s="33"/>
       <c r="C40" s="6" t="s">
         <v>39</v>
       </c>
@@ -1921,11 +1948,11 @@
       <c r="H40" s="11">
         <v>0.2</v>
       </c>
-      <c r="I40" s="39"/>
+      <c r="I40" s="40"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="35"/>
-      <c r="B41" s="32"/>
+      <c r="A41" s="36"/>
+      <c r="B41" s="33"/>
       <c r="C41" s="6" t="s">
         <v>40</v>
       </c>
@@ -1944,11 +1971,11 @@
       <c r="H41" s="11">
         <v>0.2</v>
       </c>
-      <c r="I41" s="39"/>
+      <c r="I41" s="40"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="35"/>
-      <c r="B42" s="32"/>
+      <c r="A42" s="36"/>
+      <c r="B42" s="33"/>
       <c r="C42" s="2" t="s">
         <v>14</v>
       </c>
@@ -1967,13 +1994,13 @@
       <c r="H42" s="11">
         <v>0.2</v>
       </c>
-      <c r="I42" s="39"/>
+      <c r="I42" s="40"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="35">
+      <c r="A43" s="36">
         <v>4</v>
       </c>
-      <c r="B43" s="33" t="s">
+      <c r="B43" s="34" t="s">
         <v>35</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -1994,13 +2021,13 @@
       <c r="H43" s="10">
         <v>1</v>
       </c>
-      <c r="I43" s="39">
+      <c r="I43" s="40">
         <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="35"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="2" t="s">
         <v>16</v>
       </c>
@@ -2019,11 +2046,11 @@
       <c r="H44" s="10">
         <v>1</v>
       </c>
-      <c r="I44" s="39"/>
+      <c r="I44" s="40"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="2" t="s">
         <v>17</v>
       </c>
@@ -2042,11 +2069,11 @@
       <c r="H45" s="10">
         <v>1</v>
       </c>
-      <c r="I45" s="39"/>
+      <c r="I45" s="40"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="35"/>
-      <c r="B46" s="33"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="34"/>
       <c r="C46" s="2" t="s">
         <v>18</v>
       </c>
@@ -2065,13 +2092,13 @@
       <c r="H46" s="10">
         <v>1</v>
       </c>
-      <c r="I46" s="39"/>
+      <c r="I46" s="40"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="35">
+      <c r="A47" s="36">
         <v>5</v>
       </c>
-      <c r="B47" s="33" t="s">
+      <c r="B47" s="34" t="s">
         <v>36</v>
       </c>
       <c r="C47" s="2" t="s">
@@ -2090,14 +2117,14 @@
       <c r="H47" s="10">
         <v>0.15</v>
       </c>
-      <c r="I47" s="39">
+      <c r="I47" s="40">
         <f>SUM(F47:F54)</f>
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="35"/>
-      <c r="B48" s="33"/>
+      <c r="A48" s="36"/>
+      <c r="B48" s="34"/>
       <c r="C48" s="2" t="s">
         <v>20</v>
       </c>
@@ -2114,11 +2141,11 @@
       <c r="H48" s="10">
         <v>0.1</v>
       </c>
-      <c r="I48" s="39"/>
+      <c r="I48" s="40"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="35"/>
-      <c r="B49" s="33"/>
+      <c r="A49" s="36"/>
+      <c r="B49" s="34"/>
       <c r="C49" s="2" t="s">
         <v>22</v>
       </c>
@@ -2135,11 +2162,11 @@
       <c r="H49" s="10">
         <v>0.15</v>
       </c>
-      <c r="I49" s="39"/>
+      <c r="I49" s="40"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="35"/>
-      <c r="B50" s="33"/>
+      <c r="A50" s="36"/>
+      <c r="B50" s="34"/>
       <c r="C50" s="2" t="s">
         <v>21</v>
       </c>
@@ -2156,11 +2183,11 @@
       <c r="H50" s="10">
         <v>0.1</v>
       </c>
-      <c r="I50" s="39"/>
+      <c r="I50" s="40"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="35"/>
-      <c r="B51" s="33"/>
+      <c r="A51" s="36"/>
+      <c r="B51" s="34"/>
       <c r="C51" s="2" t="s">
         <v>23</v>
       </c>
@@ -2177,11 +2204,11 @@
       <c r="H51" s="10">
         <v>0.15</v>
       </c>
-      <c r="I51" s="39"/>
+      <c r="I51" s="40"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="35"/>
-      <c r="B52" s="33"/>
+      <c r="A52" s="36"/>
+      <c r="B52" s="34"/>
       <c r="C52" s="2" t="s">
         <v>24</v>
       </c>
@@ -2198,11 +2225,11 @@
       <c r="H52" s="10">
         <v>0.1</v>
       </c>
-      <c r="I52" s="39"/>
+      <c r="I52" s="40"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="35"/>
-      <c r="B53" s="33"/>
+      <c r="A53" s="36"/>
+      <c r="B53" s="34"/>
       <c r="C53" s="2" t="s">
         <v>25</v>
       </c>
@@ -2219,11 +2246,11 @@
       <c r="H53" s="10">
         <v>0.15</v>
       </c>
-      <c r="I53" s="39"/>
+      <c r="I53" s="40"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="35"/>
-      <c r="B54" s="33"/>
+      <c r="A54" s="36"/>
+      <c r="B54" s="34"/>
       <c r="C54" s="2" t="s">
         <v>26</v>
       </c>
@@ -2240,16 +2267,16 @@
       <c r="H54" s="10">
         <v>0.1</v>
       </c>
-      <c r="I54" s="39"/>
+      <c r="I54" s="40"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>6</v>
       </c>
-      <c r="B55" s="34" t="s">
+      <c r="B55" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C55" s="34"/>
+      <c r="C55" s="35"/>
       <c r="F55" s="14">
         <v>0.3</v>
       </c>
@@ -2265,10 +2292,10 @@
       <c r="A56" s="7">
         <v>7</v>
       </c>
-      <c r="B56" s="34" t="s">
+      <c r="B56" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C56" s="34"/>
+      <c r="C56" s="35"/>
       <c r="F56" s="14">
         <v>0.5</v>
       </c>
@@ -2284,10 +2311,10 @@
       <c r="A57" s="7">
         <v>8</v>
       </c>
-      <c r="B57" s="34" t="s">
+      <c r="B57" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C57" s="34"/>
+      <c r="C57" s="35"/>
       <c r="F57" s="14">
         <v>3</v>
       </c>
@@ -2300,10 +2327,10 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="36">
+      <c r="A58" s="37">
         <v>9</v>
       </c>
-      <c r="B58" s="32" t="s">
+      <c r="B58" s="33" t="s">
         <v>57</v>
       </c>
       <c r="C58" s="3" t="s">
@@ -2321,14 +2348,14 @@
       <c r="H58" s="8">
         <v>0.1</v>
       </c>
-      <c r="I58" s="39">
+      <c r="I58" s="40">
         <f>SUM(F58:F71)</f>
         <v>1.0500000000000003</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="37"/>
-      <c r="B59" s="32"/>
+      <c r="A59" s="38"/>
+      <c r="B59" s="33"/>
       <c r="C59" s="3" t="s">
         <v>8</v>
       </c>
@@ -2344,11 +2371,11 @@
       <c r="H59" s="8">
         <v>0.1</v>
       </c>
-      <c r="I59" s="39"/>
+      <c r="I59" s="40"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="37"/>
-      <c r="B60" s="32"/>
+      <c r="A60" s="38"/>
+      <c r="B60" s="33"/>
       <c r="C60" s="3" t="s">
         <v>6</v>
       </c>
@@ -2364,11 +2391,11 @@
       <c r="H60" s="8">
         <v>0.1</v>
       </c>
-      <c r="I60" s="39"/>
+      <c r="I60" s="40"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="37"/>
-      <c r="B61" s="32"/>
+      <c r="A61" s="38"/>
+      <c r="B61" s="33"/>
       <c r="C61" s="3" t="s">
         <v>9</v>
       </c>
@@ -2384,11 +2411,11 @@
       <c r="H61" s="8">
         <v>0.1</v>
       </c>
-      <c r="I61" s="39"/>
+      <c r="I61" s="40"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="37"/>
-      <c r="B62" s="32"/>
+      <c r="A62" s="38"/>
+      <c r="B62" s="33"/>
       <c r="C62" s="3" t="s">
         <v>10</v>
       </c>
@@ -2404,11 +2431,11 @@
       <c r="H62" s="8">
         <v>0.1</v>
       </c>
-      <c r="I62" s="39"/>
+      <c r="I62" s="40"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="37"/>
-      <c r="B63" s="32"/>
+      <c r="A63" s="38"/>
+      <c r="B63" s="33"/>
       <c r="C63" s="3" t="s">
         <v>56</v>
       </c>
@@ -2424,11 +2451,11 @@
       <c r="H63" s="8">
         <v>0.05</v>
       </c>
-      <c r="I63" s="39"/>
+      <c r="I63" s="40"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="37"/>
-      <c r="B64" s="32"/>
+      <c r="A64" s="38"/>
+      <c r="B64" s="33"/>
       <c r="C64" s="9" t="s">
         <v>3</v>
       </c>
@@ -2444,11 +2471,11 @@
       <c r="H64" s="8">
         <v>0.05</v>
       </c>
-      <c r="I64" s="39"/>
+      <c r="I64" s="40"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="37"/>
-      <c r="B65" s="32"/>
+      <c r="A65" s="38"/>
+      <c r="B65" s="33"/>
       <c r="C65" s="2" t="s">
         <v>4</v>
       </c>
@@ -2464,11 +2491,11 @@
       <c r="H65" s="8">
         <v>0.05</v>
       </c>
-      <c r="I65" s="39"/>
+      <c r="I65" s="40"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="37"/>
-      <c r="B66" s="32"/>
+      <c r="A66" s="38"/>
+      <c r="B66" s="33"/>
       <c r="C66" s="2" t="s">
         <v>5</v>
       </c>
@@ -2484,11 +2511,11 @@
       <c r="H66" s="8">
         <v>0.05</v>
       </c>
-      <c r="I66" s="39"/>
+      <c r="I66" s="40"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="37"/>
-      <c r="B67" s="32"/>
+      <c r="A67" s="38"/>
+      <c r="B67" s="33"/>
       <c r="C67" s="2" t="s">
         <v>7</v>
       </c>
@@ -2504,11 +2531,11 @@
       <c r="H67" s="8">
         <v>0.1</v>
       </c>
-      <c r="I67" s="39"/>
+      <c r="I67" s="40"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="37"/>
-      <c r="B68" s="32"/>
+      <c r="A68" s="38"/>
+      <c r="B68" s="33"/>
       <c r="C68" s="2" t="s">
         <v>12</v>
       </c>
@@ -2524,11 +2551,11 @@
       <c r="H68" s="8">
         <v>0.1</v>
       </c>
-      <c r="I68" s="39"/>
+      <c r="I68" s="40"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="37"/>
-      <c r="B69" s="32"/>
+      <c r="A69" s="38"/>
+      <c r="B69" s="33"/>
       <c r="C69" s="2" t="s">
         <v>13</v>
       </c>
@@ -2544,11 +2571,11 @@
       <c r="H69" s="8">
         <v>0.05</v>
       </c>
-      <c r="I69" s="39"/>
+      <c r="I69" s="40"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="37"/>
-      <c r="B70" s="32"/>
+      <c r="A70" s="38"/>
+      <c r="B70" s="33"/>
       <c r="C70" s="6" t="s">
         <v>38</v>
       </c>
@@ -2564,11 +2591,11 @@
       <c r="H70" s="8">
         <v>0.05</v>
       </c>
-      <c r="I70" s="39"/>
+      <c r="I70" s="40"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="37"/>
-      <c r="B71" s="32"/>
+      <c r="A71" s="38"/>
+      <c r="B71" s="33"/>
       <c r="C71" s="6" t="s">
         <v>39</v>
       </c>
@@ -2584,7 +2611,7 @@
       <c r="H71" s="8">
         <v>0.05</v>
       </c>
-      <c r="I71" s="39"/>
+      <c r="I71" s="40"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
@@ -2650,6 +2677,7 @@
     <mergeCell ref="B12:B21"/>
     <mergeCell ref="B2:B11"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C36" r:id="rId1" display="http://umbrella/jqgrid/jqgrid/newpage/1/container/test_history_15677/oper/information/db/xt/table/testcase/element/15677/parent/5002157/ver/78043"/>
   </hyperlinks>
@@ -2663,84 +2691,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="42.5703125" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
+    <col min="2" max="2" width="42.54296875" customWidth="1"/>
+    <col min="3" max="3" width="4.54296875" customWidth="1"/>
+    <col min="4" max="4" width="23.453125" customWidth="1"/>
+    <col min="5" max="5" width="22.7265625" customWidth="1"/>
+    <col min="6" max="6" width="22.453125" customWidth="1"/>
+    <col min="7" max="7" width="22.1796875" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" customWidth="1"/>
+    <col min="9" max="9" width="21.54296875" customWidth="1"/>
+    <col min="10" max="10" width="22.1796875" customWidth="1"/>
     <col min="11" max="11" width="21" customWidth="1"/>
-    <col min="12" max="12" width="16.5703125" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="16.54296875" customWidth="1"/>
+    <col min="14" max="14" width="14.54296875" customWidth="1"/>
+    <col min="15" max="15" width="16.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40" t="s">
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40" t="s">
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40" t="s">
+      <c r="E2" s="41"/>
+      <c r="F2" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40" t="s">
+      <c r="G2" s="41"/>
+      <c r="H2" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40" t="s">
+      <c r="I2" s="41"/>
+      <c r="J2" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40" t="s">
+      <c r="K2" s="41"/>
+      <c r="L2" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40" t="s">
+      <c r="M2" s="41"/>
+      <c r="N2" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="40"/>
+      <c r="O2" s="41"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
       <c r="D3" s="27" t="s">
         <v>69</v>
       </c>
@@ -2779,7 +2807,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="33" t="s">
         <v>81</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -2810,7 +2838,7 @@
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -2839,7 +2867,7 @@
       <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
@@ -2868,7 +2896,7 @@
       <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
@@ -2897,7 +2925,7 @@
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
@@ -2926,7 +2954,7 @@
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="3" t="s">
         <v>29</v>
       </c>
@@ -2955,7 +2983,7 @@
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="33"/>
       <c r="B10" s="3" t="s">
         <v>75</v>
       </c>
@@ -2984,7 +3012,7 @@
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="9" t="s">
         <v>3</v>
       </c>
@@ -3029,7 +3057,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
@@ -3062,7 +3090,7 @@
       <c r="O12" s="2"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
@@ -3095,7 +3123,7 @@
       <c r="O13" s="2"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="33"/>
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
@@ -3128,7 +3156,7 @@
       <c r="O14" s="2"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
+      <c r="A15" s="33"/>
       <c r="B15" s="2" t="s">
         <v>7</v>
       </c>
@@ -3161,7 +3189,7 @@
       <c r="O15" s="2"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
+      <c r="A16" s="33"/>
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
@@ -3194,7 +3222,7 @@
       <c r="O16" s="2"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
+      <c r="A17" s="33"/>
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
@@ -3227,7 +3255,7 @@
       <c r="O17" s="2"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
+      <c r="A18" s="33"/>
       <c r="B18" s="2" t="s">
         <v>30</v>
       </c>
@@ -3260,7 +3288,7 @@
       <c r="O18" s="2"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
+      <c r="A19" s="33"/>
       <c r="B19" s="2" t="s">
         <v>27</v>
       </c>
@@ -3293,7 +3321,7 @@
       <c r="O19" s="2"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
+      <c r="A20" s="33"/>
       <c r="B20" s="9" t="s">
         <v>31</v>
       </c>
@@ -3338,7 +3366,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
+      <c r="A21" s="33"/>
       <c r="B21" s="6" t="s">
         <v>38</v>
       </c>
@@ -3371,7 +3399,7 @@
       <c r="O21" s="2"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="6" t="s">
         <v>39</v>
       </c>
@@ -3404,7 +3432,7 @@
       <c r="O22" s="2"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
+      <c r="A23" s="33"/>
       <c r="B23" s="6" t="s">
         <v>40</v>
       </c>
@@ -3429,7 +3457,7 @@
       <c r="O23" s="2"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+      <c r="A24" s="33"/>
       <c r="B24" s="2" t="s">
         <v>14</v>
       </c>
@@ -3462,10 +3490,10 @@
       <c r="C26" s="15"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="B27" s="41"/>
+      <c r="B27" s="42"/>
       <c r="C27" s="28"/>
       <c r="D27" s="27" t="s">
         <v>76</v>
@@ -3475,7 +3503,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="33" t="s">
+      <c r="A28" s="34" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -3492,7 +3520,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="33"/>
+      <c r="A29" s="34"/>
       <c r="B29" s="2" t="s">
         <v>89</v>
       </c>
@@ -3507,7 +3535,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="33"/>
+      <c r="A30" s="34"/>
       <c r="B30" s="2" t="s">
         <v>91</v>
       </c>
@@ -3522,7 +3550,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
+      <c r="A31" s="34"/>
       <c r="B31" s="2" t="s">
         <v>92</v>
       </c>
@@ -3537,7 +3565,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="34" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -3552,7 +3580,7 @@
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
+      <c r="A33" s="34"/>
       <c r="B33" s="2" t="s">
         <v>129</v>
       </c>
@@ -3565,7 +3593,7 @@
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="33"/>
+      <c r="A34" s="34"/>
       <c r="B34" s="2" t="s">
         <v>128</v>
       </c>
@@ -3578,7 +3606,7 @@
       <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="33"/>
+      <c r="A35" s="34"/>
       <c r="B35" s="2" t="s">
         <v>128</v>
       </c>
@@ -3591,7 +3619,7 @@
       <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
+      <c r="A36" s="34"/>
       <c r="B36" s="2" t="s">
         <v>129</v>
       </c>
@@ -3604,7 +3632,7 @@
       <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
+      <c r="A37" s="34"/>
       <c r="B37" s="2" t="s">
         <v>129</v>
       </c>
@@ -3617,7 +3645,7 @@
       <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
+      <c r="A38" s="34"/>
       <c r="B38" s="2" t="s">
         <v>128</v>
       </c>
@@ -3630,7 +3658,7 @@
       <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
+      <c r="A39" s="34"/>
       <c r="B39" s="2" t="s">
         <v>128</v>
       </c>
@@ -3643,7 +3671,7 @@
       <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="32" t="s">
+      <c r="A40" s="33" t="s">
         <v>57</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -3658,7 +3686,7 @@
       <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="32"/>
+      <c r="A41" s="33"/>
       <c r="B41" s="3" t="s">
         <v>8</v>
       </c>
@@ -3671,7 +3699,7 @@
       <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="32"/>
+      <c r="A42" s="33"/>
       <c r="B42" s="3" t="s">
         <v>6</v>
       </c>
@@ -3684,7 +3712,7 @@
       <c r="E42" s="2"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="32"/>
+      <c r="A43" s="33"/>
       <c r="B43" s="3" t="s">
         <v>9</v>
       </c>
@@ -3697,7 +3725,7 @@
       <c r="E43" s="2"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="32"/>
+      <c r="A44" s="33"/>
       <c r="B44" s="3" t="s">
         <v>10</v>
       </c>
@@ -3710,7 +3738,7 @@
       <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
+      <c r="A45" s="33"/>
       <c r="B45" s="3" t="s">
         <v>56</v>
       </c>
@@ -3723,7 +3751,7 @@
       <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="32"/>
+      <c r="A46" s="33"/>
       <c r="B46" s="9" t="s">
         <v>3</v>
       </c>
@@ -3736,7 +3764,7 @@
       <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="32"/>
+      <c r="A47" s="33"/>
       <c r="B47" s="2" t="s">
         <v>4</v>
       </c>
@@ -3749,7 +3777,7 @@
       <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="32"/>
+      <c r="A48" s="33"/>
       <c r="B48" s="2" t="s">
         <v>5</v>
       </c>
@@ -3762,7 +3790,7 @@
       <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+      <c r="A49" s="33"/>
       <c r="B49" s="2" t="s">
         <v>7</v>
       </c>
@@ -3775,7 +3803,7 @@
       <c r="E49" s="2"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="32"/>
+      <c r="A50" s="33"/>
       <c r="B50" s="2" t="s">
         <v>12</v>
       </c>
@@ -3788,7 +3816,7 @@
       <c r="E50" s="2"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="32"/>
+      <c r="A51" s="33"/>
       <c r="B51" s="2" t="s">
         <v>13</v>
       </c>
@@ -3801,7 +3829,7 @@
       <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="32"/>
+      <c r="A52" s="33"/>
       <c r="B52" s="6" t="s">
         <v>38</v>
       </c>
@@ -3814,7 +3842,7 @@
       <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="32"/>
+      <c r="A53" s="33"/>
       <c r="B53" s="6" t="s">
         <v>39</v>
       </c>
@@ -3825,6 +3853,17 @@
         <v>73</v>
       </c>
       <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>130</v>
+      </c>
+      <c r="B54" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="D54" s="29" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C55" s="22">
@@ -3849,6 +3888,7 @@
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="A32:A39"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B18" r:id="rId1" display="http://umbrella/jqgrid/jqgrid/newpage/1/container/test_history_15677/oper/information/db/xt/table/testcase/element/15677/parent/5002157/ver/78043"/>
   </hyperlinks>
@@ -3866,9 +3906,9 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3883,7 +3923,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="43" t="s">
         <v>56</v>
       </c>
       <c r="B6" t="s">
@@ -3891,7 +3931,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
+      <c r="A7" s="44"/>
       <c r="B7" t="s">
         <v>85</v>
       </c>
@@ -3900,6 +3940,7 @@
   <mergeCells count="1">
     <mergeCell ref="A6:A7"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>